<commit_message>
Further works on the paper
</commit_message>
<xml_diff>
--- a/data/keys_df.xlsx
+++ b/data/keys_df.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\MPIEA\projects\Dislikes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\MPIEA\projects\Dislikes\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3E5C8B-6492-4C0E-9769-820EF2CAC3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F901B39-732F-4AE0-B502-1C986AC75896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fa_keys" sheetId="1" r:id="rId1"/>
@@ -630,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5093,8 +5093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7ABA44F-6317-4B3E-84CA-096C2F839C7B}">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5110,28 +5110,28 @@
         <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>65</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -5151,7 +5151,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -5163,7 +5163,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -5215,7 +5215,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -5227,7 +5227,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -5238,7 +5238,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -5256,7 +5256,7 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -5279,7 +5279,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -5291,7 +5291,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -5302,7 +5302,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -5320,7 +5320,7 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -5337,7 +5337,7 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -5355,7 +5355,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -5366,7 +5366,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -5384,7 +5384,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -5398,7 +5398,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -5410,7 +5410,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -5433,10 +5433,10 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -5465,10 +5465,10 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -5558,7 +5558,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -5570,7 +5570,7 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -5602,13 +5602,13 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -5657,7 +5657,7 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -5675,7 +5675,7 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -5689,7 +5689,7 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -5707,7 +5707,7 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -5762,13 +5762,13 @@
         <v>0</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -5817,7 +5817,7 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -5835,7 +5835,7 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -5881,10 +5881,10 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -5977,7 +5977,7 @@
         <v>0</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -5995,7 +5995,7 @@
         <v>0</v>
       </c>
       <c r="J28">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -6006,7 +6006,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -6018,7 +6018,7 @@
         <v>0</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -6041,10 +6041,10 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -6140,10 +6140,10 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -6178,13 +6178,13 @@
         <v>0</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34">
         <v>0</v>
       </c>
       <c r="I34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34">
         <v>0</v>
@@ -6239,7 +6239,7 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -6251,7 +6251,7 @@
         <v>0</v>
       </c>
       <c r="J36">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -6326,7 +6326,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -6338,7 +6338,7 @@
         <v>0</v>
       </c>
       <c r="G39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -6361,10 +6361,10 @@
         <v>0</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -6390,7 +6390,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -6402,7 +6402,7 @@
         <v>0</v>
       </c>
       <c r="G41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -6425,10 +6425,10 @@
         <v>0</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42">
         <v>0</v>

</xml_diff>